<commit_message>
feat: Añadido botón y búsqueda Carfax style: Añadido icono Guardia Civil refactor: Creado archivo process_functions feat: añadido binding a la tecla Intro para búsqueda individual feat: cambio de buscar_modelos_carfax, aun no funciona del todo
</commit_message>
<xml_diff>
--- a/archivos/prueba1.xlsx
+++ b/archivos/prueba1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1-PROYECTOS\matriculas_GC\archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81AF3D88-45F8-40B3-9F75-C6D7DF0D5C3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966A68BC-29CB-4173-B711-7B850BA772F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3750" yWindow="2355" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,15 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Matrícula</t>
   </si>
   <si>
     <t>8909bjw</t>
-  </si>
-  <si>
-    <t>3206fvm</t>
   </si>
 </sst>
 </file>
@@ -391,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,11 +409,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>